<commit_message>
Example worksheets for Book
Example worksheets for Book C
        Title:         Continuous Testing, Quality, Security and Feedback 
        Subtitle: Mastering strategies and secure practices for DevSecOps, and SRE transformations
</commit_message>
<xml_diff>
--- a/Transformation Goals Scorecard  - Continuous Testing.xlsx
+++ b/Transformation Goals Scorecard  - Continuous Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhexc\Documents\Book - CT\Chapters\Chapter 5 - Tranformation Goals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{355BED97-115B-45A3-88C0-C62685A5642A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9DEE91-A452-475E-B6D5-DC5C93E67830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Goals Answer Sheet Template" sheetId="18" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="97">
   <si>
     <t>Agility</t>
   </si>
@@ -717,13 +717,6 @@
     <t># releases / month</t>
   </si>
   <si>
-    <t>SCORE  
-I x P%</t>
-  </si>
-  <si>
-    <t>Percent Improvement (P%)</t>
-  </si>
-  <si>
     <t>Fraction %</t>
   </si>
   <si>
@@ -754,139 +747,151 @@
     <t>The DevOps Transformation Goal Scorecard spreadsheet is posted on www.EngineeirngDevOps.com</t>
   </si>
   <si>
-    <t xml:space="preserve">c Transformation Goals Scorecard </t>
-  </si>
-  <si>
     <t>We integrate automated testing into every phase of our CI/CD pipelines.</t>
   </si>
   <si>
-    <t>We adopt test-driven development (TDD) practices across our development teams.</t>
-  </si>
-  <si>
-    <t>We implement a feature flagging system that allows us to test new features in test and production environments with select user groups.</t>
-  </si>
-  <si>
-    <t>% of pipeline phases</t>
-  </si>
-  <si>
-    <t>% of dev teams</t>
-  </si>
-  <si>
     <t>% of pipelines</t>
   </si>
   <si>
     <t>We automate our regression testing.</t>
   </si>
   <si>
-    <t>We utilize ephemeral testing environments to scale testing efforts on demand, reducing environment provisioning time.</t>
-  </si>
-  <si>
-    <t>We optimize our test automation scripts to decrease execution times, thereby increasing testing frequency without additional resource costs over the next 8 months.</t>
-  </si>
-  <si>
     <t>We implement parallel testing strategies to reduce the overall testing cycle time.</t>
   </si>
   <si>
-    <t>% regression automated</t>
-  </si>
-  <si>
     <t xml:space="preserve">Continuous Testing Transformation Goals Scorecard </t>
   </si>
   <si>
-    <t>% test environments</t>
-  </si>
-  <si>
     <t>% of scripts</t>
   </si>
   <si>
-    <t>% of test suites</t>
-  </si>
-  <si>
-    <t>We ensure reduced downtime due to testing environment issues by implementing automated health checks and recovery processes.</t>
-  </si>
-  <si>
     <t>% uptime</t>
   </si>
   <si>
-    <t>We achieve high %uptime of our continuous testing infrastructure, ensuring testing operations are uninterrupted.</t>
-  </si>
-  <si>
-    <t>We increase the defect detection rate before code reaches the production environment, leveraging automated and manual testing synergies.</t>
-  </si>
-  <si>
-    <t>We improve user satisfaction scores by integrating continuous user experience testing into our release process.</t>
-  </si>
-  <si>
-    <t>We conduct bi-weekly quality audits on our testing processes, aiming for improvement in our internal quality metrics quarter over quarter.</t>
-  </si>
-  <si>
-    <t># of defects found before release.</t>
-  </si>
-  <si>
-    <t># issues per release</t>
-  </si>
-  <si>
-    <t># fixes</t>
-  </si>
-  <si>
-    <t>We reduce # of production hotfixes per release required through enhanced early detection of issues in the testing phase within the next year.</t>
-  </si>
-  <si>
     <t>We reduce the % of release rollbacks for all deployments.</t>
   </si>
   <si>
     <t>1.0 to 10.0</t>
   </si>
   <si>
-    <t>Increase coverage of critical user journeys with automated tests, reduces user-reported issues.</t>
-  </si>
-  <si>
     <t>We integrate automated security testing into every stage of our CI/CD pipelines.</t>
   </si>
   <si>
-    <t>We test for compliance with our security compliance requirements for our releases, reducing security-related incidents.</t>
-  </si>
-  <si>
-    <t>We conduct quarterly security training for our development and QA teams, aiming to reduce security breaches due to human error.</t>
-  </si>
-  <si>
-    <t>We implement continuous monitoring for security vulnerabilities in third-party dependencies, reducing the risk exposure time.</t>
-  </si>
-  <si>
     <t>% of stages</t>
   </si>
   <si>
-    <t>% of compliance reqts covered</t>
-  </si>
-  <si>
     <t>% of teams</t>
   </si>
   <si>
-    <t>We establish a continuous learning culture, with the team receiving certification in automated testing tools within the next year.</t>
-  </si>
-  <si>
-    <t>We increase team engagement scores by introducing a mentorship program pairing junior and senior professionals.</t>
-  </si>
-  <si>
-    <t>We recognize and reward contributions to testing excellence monthly, leading to an increase in innovative testing practices adopted by the team.</t>
-  </si>
-  <si>
-    <t>% certified</t>
-  </si>
-  <si>
-    <t>We increase the satisfaction score among our development and QA teams regarding the support and resources for continuous testing.</t>
-  </si>
-  <si>
     <t>% satisfied</t>
   </si>
   <si>
-    <t>% Engagement</t>
-  </si>
-  <si>
-    <t>We increase the % of  developed features that have associated automated tests before merging into the main branch, enhancing our test coverage.</t>
-  </si>
-  <si>
-    <t>% of features</t>
+    <t>SCORE  (I x P%)</t>
+  </si>
+  <si>
+    <t># of fixes</t>
+  </si>
+  <si>
+    <t># of hours</t>
+  </si>
+  <si>
+    <t>We adopt Test-Driven Development (TDD) practices across our development teams.</t>
+  </si>
+  <si>
+    <t>We automate testing of critical user journeys to reduce user-reported issues.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importance </t>
+  </si>
+  <si>
+    <t>Percent Improvement</t>
+  </si>
+  <si>
+    <t>We increase the satisfaction score  regarding the support and resources for continuous testing.</t>
+  </si>
+  <si>
+    <t>We increase team engagement scores by introducing a mentorship program.</t>
+  </si>
+  <si>
+    <t>% engaged</t>
+  </si>
+  <si>
+    <t>We recognize and reward contributions to testing excellence.</t>
+  </si>
+  <si>
+    <t>% trained</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We establish a continuous learning culture, and training in continuous testing. </t>
+  </si>
+  <si>
+    <t>We scan for security vulnerabilities in third-party dependencies.</t>
+  </si>
+  <si>
+    <t>%  pipelines</t>
+  </si>
+  <si>
+    <t>We conduct quarterly security training  to reduce security breaches due to human error.</t>
+  </si>
+  <si>
+    <t>We test for compliance with our security compliance requirements for our releases.</t>
+  </si>
+  <si>
+    <t>% compliance</t>
+  </si>
+  <si>
+    <t>We conduct bi-weekly quality audits on our testing processes.</t>
+  </si>
+  <si>
+    <t>%  journeys</t>
+  </si>
+  <si>
+    <t>We iintegrate continuous user experience testing into our release process.</t>
+  </si>
+  <si>
+    <t>% /release</t>
+  </si>
+  <si>
+    <t>We use continuous testing automated and manual testing to reduce detects.</t>
+  </si>
+  <si>
+    <t>% rollbacks</t>
+  </si>
+  <si>
+    <t>We  reduce downtime to testing environmentss using automated health checks and recovery.</t>
+  </si>
+  <si>
+    <t>We reduce # of production hotfixes per release.</t>
+  </si>
+  <si>
+    <t>We achieve high %uptime of our continuous testing infrastructure.</t>
+  </si>
+  <si>
+    <t>%  test suites</t>
+  </si>
+  <si>
+    <t>We optimize our test automation scripts to decrease execution times.</t>
+  </si>
+  <si>
+    <t>We utilize ephemeral testing environments to scale testing efforts on demand.</t>
+  </si>
+  <si>
+    <t>% environments</t>
+  </si>
+  <si>
+    <t>% regression</t>
+  </si>
+  <si>
+    <t>We automate tests for new features  before merging a  feature into the main branch.</t>
+  </si>
+  <si>
+    <t>%  automated</t>
+  </si>
+  <si>
+    <t>We use feature flagging   in test and production environments.</t>
+  </si>
+  <si>
+    <t>% of phases</t>
   </si>
 </sst>
 </file>
@@ -1049,7 +1054,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1128,9 +1133,6 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1200,6 +1202,18 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1759,22 +1773,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.6328125" style="27" customWidth="1"/>
+    <col min="1" max="1" width="51.6328125" style="26" customWidth="1"/>
     <col min="2" max="2" width="10.36328125" style="16" customWidth="1"/>
     <col min="3" max="3" width="11.90625" style="2" customWidth="1"/>
     <col min="4" max="5" width="8.26953125" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.36328125" style="1" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="27" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" s="26" customFormat="1" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>44</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>11</v>
@@ -1816,76 +1830,76 @@
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33" t="e">
+      <c r="C5" s="30"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32" t="e">
         <f>IF(C5="y",1,0)*(D5-E5)/E5</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33" t="e">
+      <c r="C6" s="30"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="32" t="e">
         <f>IF(C6="y",1,0)*(E6-D6)/D6</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="49.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="33" t="e">
+      <c r="B7" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="32" t="e">
         <f>IF(C7="y",1,0)*(E7-D7)/D7</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="39.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33" t="e">
+      <c r="C8" s="30"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32" t="e">
         <f t="shared" ref="F8" si="0">IF(C8="y",1,0)*(E8-D8)/D8</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33" t="e">
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32" t="e">
         <f>IF(C9="y",1,0)*(E9-D9)/D9</f>
         <v>#DIV/0!</v>
       </c>
@@ -1920,46 +1934,46 @@
       <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="33">
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="32">
         <f>IF(C13="y",1,0)*(IFERROR((D13-E13)/E13,((D13+1)-(E13+1)/(E13+1))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="33">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="32">
         <f>IF(C14="y",1,0)*(IFERROR((D14-E14)/E14,((D14+1)-(E14+1)/(E14+1))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="33" t="e">
+      <c r="C15" s="30"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="32" t="e">
         <f>IF(C15="y",1,0)*(D15-E15)/E15</f>
         <v>#DIV/0!</v>
       </c>
@@ -1994,61 +2008,61 @@
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="44.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33" t="e">
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32" t="e">
         <f>IF(C19="y",1,0)*(E19-D19)/D19</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33" t="e">
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32" t="e">
         <f t="shared" ref="F20:F22" si="1">IF(C20="y",1,0)*(E20-D20)/D20</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33" t="e">
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33" t="e">
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -2083,31 +2097,31 @@
       <c r="F25" s="10"/>
     </row>
     <row r="26" spans="1:6" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33" t="e">
+      <c r="C26" s="30"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32" t="e">
         <f>IF(C26="y",1,0)*(D26-E26)/E26</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="33" t="e">
+      <c r="C27" s="30"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="32" t="e">
         <f>IF(C27="y",1,0)*(D27-E27)/E27</f>
         <v>#DIV/0!</v>
       </c>
@@ -2142,46 +2156,46 @@
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="33">
+      <c r="C31" s="30"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="32">
         <f>IF(C31="y",1,0)*(IFERROR((D31-E31)/E31,((D31+1)-(E31+1))/(E31+1)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="45.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33" t="e">
+      <c r="C32" s="30"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="32" t="e">
         <f>IF(C32="y",1,0)*(E32-D32)/D32</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33" t="e">
+      <c r="C33" s="30"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32" t="e">
         <f>IF(C33="y",1,0)*(E33-D33)/D33</f>
         <v>#DIV/0!</v>
       </c>
@@ -2216,61 +2230,61 @@
       <c r="F36" s="10"/>
     </row>
     <row r="37" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="33" t="e">
+      <c r="C37" s="30"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="32" t="e">
         <f>IF(C37="y",1,0)*(D37-E37)/E37</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="40.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="33" t="e">
+      <c r="C38" s="30"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="32" t="e">
         <f t="shared" ref="F38" si="2">IF(C38="y",1,0)*(E38-D38)/D38</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="41.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33" t="e">
+      <c r="C39" s="30"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="32" t="e">
         <f>IF(C39="y",1,0)*(#REF!-D39)/D39</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="33" t="e">
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="32" t="e">
         <f t="shared" ref="F40" si="3">IF(C40="y",1,0)*(E40-D40)/D40</f>
         <v>#DIV/0!</v>
       </c>
@@ -2284,11 +2298,11 @@
       <c r="F41" s="6"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="48"/>
-      <c r="B43" s="49"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
+      <c r="A43" s="51"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2322,56 +2336,55 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.81640625" style="27" customWidth="1"/>
-    <col min="2" max="2" width="13.08984375" style="45" customWidth="1"/>
-    <col min="3" max="3" width="13.90625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="9.6328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="80.6328125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" style="44" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.08984375" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.453125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.26953125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.6328125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="7" style="2" customWidth="1"/>
+    <col min="8" max="8" width="5.08984375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="5.26953125" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="27" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" s="26" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="26" t="s">
+      <c r="G1" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="50" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="5.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="41"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2384,7 +2397,7 @@
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="42"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="21">
         <f>IFERROR(AVERAGE(C4:C9),"")</f>
         <v>4</v>
@@ -2399,18 +2412,18 @@
         <f>IFERROR(AVERAGE(G4:G9),"")</f>
         <v>2.0059523809523809</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="34">
         <f>IFERROR(C3*G3,"")</f>
         <v>8.0238095238095237</v>
       </c>
-      <c r="I3" s="36">
+      <c r="I3" s="35">
         <f>IFERROR(RANK(H3,(H$3,H$10,H$17,H$24,H$31,H$38)),"")</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
-      <c r="B4" s="43"/>
+      <c r="B4" s="42"/>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -2419,141 +2432,141 @@
       <c r="H4" s="9"/>
       <c r="I4" s="25"/>
     </row>
-    <row r="5" spans="1:9" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="31">
+    <row r="5" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="30">
         <v>5</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="39">
         <v>0.2</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="39">
         <v>0.9</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <f>IF(C5="y",1,0)*(D5-E5)/E5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="33">
         <f>(E5-D5)/D5</f>
         <v>3.4999999999999996</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="34">
         <f>IFERROR(C5*G5,"")</f>
         <v>17.499999999999996</v>
       </c>
-      <c r="I5" s="36">
+      <c r="I5" s="35">
         <f>IFERROR(RANK(H5,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="31">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="30">
         <v>4</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="39">
         <v>0.3</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="39">
         <v>0.8</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="32">
         <f>IF(C6="y",1,0)*(E6-D6)/D6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="33">
         <f t="shared" ref="G6:G8" si="0">(E6-D6)/D6</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="34">
         <f t="shared" ref="H6:H7" si="1">IFERROR(C6*G6,"")</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="I6" s="36">
+      <c r="I6" s="35">
         <f>IFERROR(RANK(H6,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="31">
+    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="30">
         <v>4</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="33">
         <v>0.25</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="33">
         <v>0.75</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <f>IF(C7="y",1,0)*(E7-D7)/D7</f>
         <v>0</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="34">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="35">
         <f>IFERROR(RANK(H7,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>3</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="33">
         <v>0.35</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <v>0.65</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <f>IF(C8="y",1,0)*(E8-D8)/D8</f>
         <v>0</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="33">
         <f t="shared" si="0"/>
         <v>0.85714285714285732</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="34">
         <f t="shared" ref="H8" si="2">IFERROR(C8*G8,"")</f>
         <v>2.5714285714285721</v>
       </c>
-      <c r="I8" s="36">
+      <c r="I8" s="35">
         <f>IFERROR(RANK(H8,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
-      <c r="B9" s="43"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -2566,7 +2579,7 @@
       <c r="A10" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="42"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="21">
         <f>IFERROR(AVERAGE(C11:C16),"")</f>
         <v>3.5</v>
@@ -2581,18 +2594,18 @@
         <f>IFERROR(AVERAGE(G11:G16),"")</f>
         <v>1.0333333333333332</v>
       </c>
-      <c r="H10" s="35">
+      <c r="H10" s="34">
         <f>IFERROR(C10*G10,"")</f>
         <v>3.6166666666666663</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="35">
         <f>IFERROR(RANK(H10,(H$3,H$10,H$17,H$24,H$31,H$38)),"")</f>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
-      <c r="B11" s="43"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -2601,141 +2614,141 @@
       <c r="H11" s="9"/>
       <c r="I11" s="25"/>
     </row>
-    <row r="12" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="31">
+    <row r="12" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="30">
         <v>4</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="33">
         <v>0.5</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="33">
         <v>0.9</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <f>IF(C12="y",1,0)*(D12-E12)/E12</f>
         <v>0</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="33">
         <f>(E12-D12)/D12</f>
         <v>0.8</v>
       </c>
-      <c r="H12" s="35">
+      <c r="H12" s="34">
         <f t="shared" ref="H12:H15" si="3">IFERROR(C12*G12,"")</f>
         <v>3.2</v>
       </c>
-      <c r="I12" s="36">
+      <c r="I12" s="35">
         <f>IFERROR(RANK(H12,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="40.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="31">
+    <row r="13" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="30">
         <v>4</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="39">
         <v>0.3</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="39">
         <v>0.7</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <f t="shared" ref="F13" si="4">IF(C13="y",1,0)*(E13-D13)/D13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="33">
         <f t="shared" ref="G13:G15" si="5">(E13-D13)/D13</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="34">
         <f t="shared" si="3"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="I13" s="36">
+      <c r="I13" s="35">
         <f>IFERROR(RANK(H13,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="41.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="31">
+    <row r="14" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="30">
         <v>3</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="39">
         <v>0.25</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="39">
         <v>0.5</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <f>IF(C14="y",1,0)*(G10-D14)/D14</f>
         <v>0</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="33">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="H14" s="35">
+      <c r="H14" s="34">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I14" s="36">
+      <c r="I14" s="35">
         <f>IFERROR(RANK(H14,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="31">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="30">
         <v>3</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="39">
         <v>0.25</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="39">
         <v>0.5</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="32">
         <f t="shared" ref="F15" si="6">IF(C15="y",1,0)*(E15-D15)/D15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="33">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="H15" s="35">
+      <c r="H15" s="34">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I15" s="36">
+      <c r="I15" s="35">
         <f>IFERROR(RANK(H15,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
-      <c r="B16" s="43"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -2748,7 +2761,7 @@
       <c r="A17" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="42"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="21">
         <f>IFERROR(AVERAGE(C18:C23),"")</f>
         <v>4</v>
@@ -2763,18 +2776,18 @@
         <f>IFERROR(AVERAGE(G18:G23),"")</f>
         <v>0.42083333333333334</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="34">
         <f>IFERROR(C17*G17,"")</f>
         <v>1.6833333333333333</v>
       </c>
-      <c r="I17" s="36">
+      <c r="I17" s="35">
         <f>IFERROR(RANK(H17,(H$3,H$10,H$17,H$24,H$31,H$38)),"")</f>
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
-      <c r="B18" s="43"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -2783,141 +2796,141 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="31">
+    <row r="19" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="30">
         <v>4</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="33">
         <v>0.6</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="33">
         <v>0.9</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="32">
         <f>IF(C19="y",1,0)*(D19-E19)/E19</f>
         <v>0</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="46">
         <f t="shared" ref="G19" si="7">(E19-D19)/D19</f>
         <v>0.50000000000000011</v>
       </c>
-      <c r="H19" s="35">
+      <c r="H19" s="34">
         <f t="shared" ref="H19:H20" si="8">IFERROR(C19*G19,"")</f>
         <v>2.0000000000000004</v>
       </c>
-      <c r="I19" s="36">
+      <c r="I19" s="35">
         <f>IFERROR(RANK(H19,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C20" s="31">
+    <row r="20" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="30">
         <v>4</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="30">
         <v>10</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="30">
         <v>5</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="32">
         <f>IF(C20="y",1,0)*(D20-E20)/E20</f>
         <v>0</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="33">
         <f>(D20-E20)/D20</f>
         <v>0.5</v>
       </c>
-      <c r="H20" s="35">
+      <c r="H20" s="34">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="I20" s="36">
+      <c r="I20" s="35">
         <f>IFERROR(RANK(H20,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="31">
+    <row r="21" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="30">
         <v>4</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="33">
         <v>1</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="33">
         <v>0.65</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="32">
         <f>IF(C21="y",1,0)*(D21-E21)/E21</f>
         <v>0</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="33">
         <f>(D21-E21)/D21</f>
         <v>0.35</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H21" s="34">
         <f t="shared" ref="H21:H22" si="9">IFERROR(C21*G21,"")</f>
         <v>1.4</v>
       </c>
-      <c r="I21" s="36">
+      <c r="I21" s="35">
         <f>IFERROR(RANK(H21,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="31">
+    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="30">
         <v>4</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="33">
         <v>0.15</v>
       </c>
-      <c r="E22" s="34">
+      <c r="E22" s="33">
         <v>0.1</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="32">
         <f>IF(C22="y",1,0)*(D22-E22)/E22</f>
         <v>0</v>
       </c>
-      <c r="G22" s="34">
+      <c r="G22" s="33">
         <f>(D22-E22)/D22</f>
         <v>0.33333333333333326</v>
       </c>
-      <c r="H22" s="35">
+      <c r="H22" s="34">
         <f t="shared" si="9"/>
         <v>1.333333333333333</v>
       </c>
-      <c r="I22" s="36">
+      <c r="I22" s="35">
         <f>IFERROR(RANK(H22,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
-      <c r="B23" s="43"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -2930,7 +2943,7 @@
       <c r="A24" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="42"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="21">
         <f>IFERROR(AVERAGE(C25:C30),"")</f>
         <v>3.75</v>
@@ -2945,18 +2958,18 @@
         <f>IFERROR(AVERAGE(G25:G30),"")</f>
         <v>0.44523809523809521</v>
       </c>
-      <c r="H24" s="35">
+      <c r="H24" s="34">
         <f>IFERROR(C24*G24,"")</f>
         <v>1.669642857142857</v>
       </c>
-      <c r="I24" s="36">
+      <c r="I24" s="35">
         <f>IFERROR(RANK(H24,(H$3,H$10,H$17,H$24,H$31,H$38)),"")</f>
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
-      <c r="B25" s="43"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -2965,141 +2978,141 @@
       <c r="H25" s="9"/>
       <c r="I25" s="25"/>
     </row>
-    <row r="26" spans="1:9" ht="44" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="31">
+    <row r="26" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="30">
         <v>4</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="33">
         <v>0.75</v>
       </c>
-      <c r="E26" s="34">
+      <c r="E26" s="33">
         <v>0.95</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="32">
         <f>IF(C26="y",1,0)*(IFERROR((D26-E26)/E26,((D26+1)-(E26+1))/(E26+1)))</f>
         <v>0</v>
       </c>
-      <c r="G26" s="34">
+      <c r="G26" s="33">
         <f t="shared" ref="G26:G29" si="10">(E26-D26)/D26</f>
         <v>0.26666666666666661</v>
       </c>
-      <c r="H26" s="35">
+      <c r="H26" s="34">
         <f t="shared" ref="H26:H29" si="11">IFERROR(C26*G26,"")</f>
         <v>1.0666666666666664</v>
       </c>
-      <c r="I26" s="36">
+      <c r="I26" s="35">
         <f>IFERROR(RANK(H26,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="31">
+    <row r="27" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="30">
         <v>4</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="31">
         <v>7</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="31">
         <v>8.5</v>
       </c>
-      <c r="F27" s="33">
+      <c r="F27" s="32">
         <f>IF(C27="y",1,0)*(E27-D27)/D27</f>
         <v>0</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="33">
         <f t="shared" si="10"/>
         <v>0.21428571428571427</v>
       </c>
-      <c r="H27" s="35">
+      <c r="H27" s="34">
         <f t="shared" ref="H27" si="12">IFERROR(C27*G27,"")</f>
         <v>0.8571428571428571</v>
       </c>
-      <c r="I27" s="36">
+      <c r="I27" s="35">
         <f>IFERROR(RANK(H27,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="45.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="31">
+    <row r="28" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="30">
         <v>4</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="33">
         <v>0.5</v>
       </c>
-      <c r="E28" s="34">
+      <c r="E28" s="33">
         <v>0.65</v>
       </c>
-      <c r="F28" s="33">
+      <c r="F28" s="32">
         <f>IF(C28="y",1,0)*(E28-D28)/D28</f>
         <v>0</v>
       </c>
-      <c r="G28" s="34">
+      <c r="G28" s="33">
         <f t="shared" si="10"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="34">
         <f t="shared" si="11"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="I28" s="36">
+      <c r="I28" s="35">
         <f>IFERROR(RANK(H28,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="38.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="31">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="30">
         <v>3</v>
       </c>
-      <c r="D29" s="34">
+      <c r="D29" s="33">
         <v>0.25</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="33">
         <v>0.5</v>
       </c>
-      <c r="F29" s="33">
+      <c r="F29" s="32">
         <f>IF(C29="y",1,0)*(E29-D29)/D29</f>
         <v>0</v>
       </c>
-      <c r="G29" s="34">
+      <c r="G29" s="33">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="H29" s="35">
+      <c r="H29" s="34">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="I29" s="36">
+      <c r="I29" s="35">
         <f>IFERROR(RANK(H29,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="7"/>
-      <c r="B30" s="43"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
@@ -3112,7 +3125,7 @@
       <c r="A31" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="42"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="21">
         <f>IFERROR(AVERAGE(C32:C37),"")</f>
         <v>4.5</v>
@@ -3127,18 +3140,18 @@
         <f>IFERROR(AVERAGE(G32:G37),"")</f>
         <v>1.2134920634920636</v>
       </c>
-      <c r="H31" s="35">
+      <c r="H31" s="34">
         <f>IFERROR(C31*G31,"")</f>
         <v>5.4607142857142863</v>
       </c>
-      <c r="I31" s="36">
+      <c r="I31" s="35">
         <f>IFERROR(RANK(H31,(H$3,H$10,H$17,H$24,H$31,H$38)),"")</f>
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="7"/>
-      <c r="B32" s="43"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -3147,141 +3160,141 @@
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
     </row>
-    <row r="33" spans="1:9" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="31">
+    <row r="33" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="30">
         <v>4</v>
       </c>
-      <c r="D33" s="34">
+      <c r="D33" s="33">
         <v>0.5</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="33">
         <v>0.8</v>
       </c>
-      <c r="F33" s="33">
+      <c r="F33" s="32">
         <f>IF(C33="y",1,0)*(IFERROR((D33-E33)/E33,((D33+1)-(E33+1)/(E33+1))))</f>
         <v>0</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="33">
         <f t="shared" ref="G33:G36" si="13">(E33-D33)/D33</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="H33" s="35">
+      <c r="H33" s="34">
         <f t="shared" ref="H33:H36" si="14">IFERROR(C33*G33,"")</f>
         <v>2.4000000000000004</v>
       </c>
-      <c r="I33" s="36">
+      <c r="I33" s="35">
         <f>IFERROR(RANK(H33,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="31">
+    <row r="34" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="30">
         <v>5</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34" s="33">
         <v>0.45</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="33">
         <v>0.95</v>
       </c>
-      <c r="F34" s="33">
+      <c r="F34" s="32">
         <f>IF(C34="y",1,0)*(IFERROR((D34-E34)/E34,((D34+1)-(E34+1)/(E34+1))))</f>
         <v>0</v>
       </c>
-      <c r="G34" s="34">
+      <c r="G34" s="33">
         <f t="shared" si="13"/>
         <v>1.1111111111111109</v>
       </c>
-      <c r="H34" s="35">
+      <c r="H34" s="34">
         <f t="shared" ref="H34" si="15">IFERROR(C34*G34,"")</f>
         <v>5.5555555555555545</v>
       </c>
-      <c r="I34" s="36">
+      <c r="I34" s="35">
         <f>IFERROR(RANK(H34,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="31">
+    <row r="35" spans="1:9" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="30">
         <v>5</v>
       </c>
-      <c r="D35" s="34">
+      <c r="D35" s="33">
         <v>0.35</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="33">
         <v>0.9</v>
       </c>
-      <c r="F35" s="33">
+      <c r="F35" s="32">
         <f>IF(C35="y",1,0)*(IFERROR((D35-E35)/E35,((D35+1)-(E35+1)/(E35+1))))</f>
         <v>0</v>
       </c>
-      <c r="G35" s="34">
+      <c r="G35" s="33">
         <f t="shared" si="13"/>
         <v>1.5714285714285716</v>
       </c>
-      <c r="H35" s="35">
+      <c r="H35" s="34">
         <f t="shared" si="14"/>
         <v>7.8571428571428577</v>
       </c>
-      <c r="I35" s="36">
+      <c r="I35" s="35">
         <f>IFERROR(RANK(H35,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="31">
+    <row r="36" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="30">
         <v>4</v>
       </c>
-      <c r="D36" s="34">
+      <c r="D36" s="33">
         <v>0.35</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="33">
         <v>0.9</v>
       </c>
-      <c r="F36" s="33">
+      <c r="F36" s="32">
         <f>IF(C36="y",1,0)*(D36-E36)/E36</f>
         <v>0</v>
       </c>
-      <c r="G36" s="34">
+      <c r="G36" s="33">
         <f t="shared" si="13"/>
         <v>1.5714285714285716</v>
       </c>
-      <c r="H36" s="35">
+      <c r="H36" s="34">
         <f t="shared" si="14"/>
         <v>6.2857142857142865</v>
       </c>
-      <c r="I36" s="36">
+      <c r="I36" s="35">
         <f>IFERROR(RANK(H36,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="7"/>
-      <c r="B37" s="43"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -3294,7 +3307,7 @@
       <c r="A38" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="42"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="21">
         <f>IFERROR(AVERAGE(C39:C44),"")</f>
         <v>3.75</v>
@@ -3309,18 +3322,18 @@
         <f>IFERROR(AVERAGE(G39:G44),"")</f>
         <v>0.88194444444444442</v>
       </c>
-      <c r="H38" s="35">
+      <c r="H38" s="34">
         <f>IFERROR(C38*G38,"")</f>
         <v>3.3072916666666665</v>
       </c>
-      <c r="I38" s="36">
+      <c r="I38" s="35">
         <f>IFERROR(RANK(H38,(H$3,H$10,H$17,H$24,H$31,H$38)),"")</f>
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7"/>
-      <c r="B39" s="43"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -3329,141 +3342,141 @@
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
     </row>
-    <row r="40" spans="1:9" ht="44.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="31">
+    <row r="40" spans="1:9" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="30">
         <v>3</v>
       </c>
-      <c r="D40" s="34">
+      <c r="D40" s="33">
         <v>0.3</v>
       </c>
-      <c r="E40" s="34">
+      <c r="E40" s="33">
         <v>0.6</v>
       </c>
-      <c r="F40" s="33">
+      <c r="F40" s="32">
         <f>IF(C40="y",1,0)*(E40-D40)/D40</f>
         <v>0</v>
       </c>
-      <c r="G40" s="34">
+      <c r="G40" s="33">
         <f t="shared" ref="G40:G42" si="16">(E40-D40)/D40</f>
         <v>1</v>
       </c>
-      <c r="H40" s="35">
+      <c r="H40" s="34">
         <f t="shared" ref="H40:H43" si="17">IFERROR(C40*G40,"")</f>
         <v>3</v>
       </c>
-      <c r="I40" s="36">
+      <c r="I40" s="35">
         <f>IFERROR(RANK(H40,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="31">
+    <row r="41" spans="1:9" ht="21.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="30">
         <v>4</v>
       </c>
-      <c r="D41" s="34">
+      <c r="D41" s="33">
         <v>0.4</v>
       </c>
-      <c r="E41" s="34">
+      <c r="E41" s="33">
         <v>0.7</v>
       </c>
-      <c r="F41" s="33">
+      <c r="F41" s="32">
         <f t="shared" ref="F41:F42" si="18">IF(C41="y",1,0)*(E41-D41)/D41</f>
         <v>0</v>
       </c>
-      <c r="G41" s="34">
+      <c r="G41" s="33">
         <f t="shared" si="16"/>
         <v>0.74999999999999978</v>
       </c>
-      <c r="H41" s="35">
+      <c r="H41" s="34">
         <f t="shared" si="17"/>
         <v>2.9999999999999991</v>
       </c>
-      <c r="I41" s="36">
+      <c r="I41" s="35">
         <f>IFERROR(RANK(H41,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="31">
+    <row r="42" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="30">
         <v>4</v>
       </c>
-      <c r="D42" s="34">
+      <c r="D42" s="33">
         <v>0.45</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="33">
         <v>0.8</v>
       </c>
-      <c r="F42" s="33">
+      <c r="F42" s="32">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="G42" s="34">
+      <c r="G42" s="33">
         <f t="shared" si="16"/>
         <v>0.77777777777777779</v>
       </c>
-      <c r="H42" s="35">
+      <c r="H42" s="34">
         <f t="shared" si="17"/>
         <v>3.1111111111111112</v>
       </c>
-      <c r="I42" s="36">
+      <c r="I42" s="35">
         <f>IFERROR(RANK(H42,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="31">
+    <row r="43" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="30">
         <v>4</v>
       </c>
-      <c r="D43" s="34">
+      <c r="D43" s="33">
         <v>0.3</v>
       </c>
-      <c r="E43" s="34">
+      <c r="E43" s="33">
         <v>0.6</v>
       </c>
-      <c r="F43" s="33">
+      <c r="F43" s="32">
         <f t="shared" ref="F43" si="19">IF(C43="y",1,0)*(E43-D43)/D43</f>
         <v>0</v>
       </c>
-      <c r="G43" s="34">
+      <c r="G43" s="33">
         <f t="shared" ref="G43" si="20">(E43-D43)/D43</f>
         <v>1</v>
       </c>
-      <c r="H43" s="35">
+      <c r="H43" s="34">
         <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="I43" s="36">
+      <c r="I43" s="35">
         <f>IFERROR(RANK(H43,(H$4:H$9,H$11:H$16,H$18:H$23,H$25:H$30,H$32:H$37,H$39:H$44)),"")</f>
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="5.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
-      <c r="B44" s="43"/>
+      <c r="B44" s="42"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -3474,7 +3487,7 @@
     </row>
     <row r="45" spans="1:9" ht="7.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -3484,18 +3497,18 @@
       <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="27" t="s">
-        <v>48</v>
+      <c r="A46" s="26" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A47" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
+      <c r="A47" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="52"/>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>